<commit_message>
adding a few more testcases
</commit_message>
<xml_diff>
--- a/com.chase/src/main/resources/ChaseTestData.xlsx
+++ b/com.chase/src/main/resources/ChaseTestData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erdosa\IdeaProjects\Selenium_Framework_Team2\com.chase\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86739C2C-9806-423C-A567-00FB94F0987E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395B45F5-117B-4C8D-97F0-A0D35503FFD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{2E8A104B-F2B9-46B0-BA3D-725330091B04}"/>
+    <workbookView xWindow="5115" yWindow="720" windowWidth="15375" windowHeight="7005" firstSheet="2" activeTab="3" xr2:uid="{2E8A104B-F2B9-46B0-BA3D-725330091B04}"/>
   </bookViews>
   <sheets>
     <sheet name="BusinessSolutions" sheetId="2" r:id="rId1"/>
     <sheet name="CarouselLinksTitles" sheetId="3" r:id="rId2"/>
     <sheet name="TabsCompareAccounts" sheetId="6" r:id="rId3"/>
+    <sheet name="FirstBankingLinks" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>An all-in-one business checking solution</t>
   </si>
@@ -82,6 +83,15 @@
   <si>
     <t>Premium
 updates page content</t>
+  </si>
+  <si>
+    <t>Chase First Banking: a debit card for teens and kids, managed by parents</t>
+  </si>
+  <si>
+    <t>FAQs | Chase First Banking: child-friendly bank account opened by parents</t>
+  </si>
+  <si>
+    <t>Chase First Banking vs. Chase High School Checking student accounts | Chase</t>
   </si>
 </sst>
 </file>
@@ -471,7 +481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7494D8B3-9FC9-4CAC-A07A-81A91BD1621E}">
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -599,7 +609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB492D8-F205-4B44-A119-44F47A29C50F}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -631,4 +641,44 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA1DC26-0AF3-4993-9A5D-6AD2C6B2DE93}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>